<commit_message>
SOme minor refinements to the lsmeans calculations and export functions
</commit_message>
<xml_diff>
--- a/exports/yield_files/LO-HP 6.xlsx
+++ b/exports/yield_files/LO-HP 6.xlsx
@@ -6508,46 +6508,36 @@
         <v>7</v>
       </c>
       <c r="F108" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G108" t="n">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H108"/>
       <c r="I108"/>
-      <c r="J108" t="n">
-        <v>18</v>
-      </c>
+      <c r="J108"/>
       <c r="K108" t="s">
         <v>52</v>
       </c>
-      <c r="L108" t="s">
-        <v>28</v>
-      </c>
-      <c r="M108" t="n">
-        <v>30</v>
-      </c>
-      <c r="N108" t="n">
-        <v>1</v>
-      </c>
+      <c r="L108"/>
+      <c r="M108"/>
+      <c r="N108"/>
       <c r="O108" t="n">
-        <v>20.46</v>
+        <v>20.37</v>
       </c>
       <c r="P108" t="n">
-        <v>47</v>
+        <v>46.76</v>
       </c>
       <c r="Q108" t="n">
-        <v>67.46</v>
+        <v>67.13</v>
       </c>
       <c r="R108" t="n">
-        <v>2310.2</v>
+        <v>2151.8</v>
       </c>
       <c r="S108" t="n">
-        <v>16.8</v>
-      </c>
-      <c r="T108" t="n">
-        <v>1.5</v>
-      </c>
+        <v>15.5</v>
+      </c>
+      <c r="T108"/>
       <c r="U108" t="n">
         <v>55.9</v>
       </c>
@@ -6569,10 +6559,10 @@
         <v>7</v>
       </c>
       <c r="F109" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G109" t="n">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="H109"/>
       <c r="I109"/>
@@ -6583,24 +6573,18 @@
       <c r="L109"/>
       <c r="M109"/>
       <c r="N109"/>
-      <c r="O109" t="n">
-        <v>20.37</v>
-      </c>
-      <c r="P109" t="n">
-        <v>46.76</v>
-      </c>
-      <c r="Q109" t="n">
-        <v>67.13</v>
-      </c>
+      <c r="O109"/>
+      <c r="P109"/>
+      <c r="Q109"/>
       <c r="R109" t="n">
-        <v>2151.8</v>
+        <v>2023.9</v>
       </c>
       <c r="S109" t="n">
-        <v>15.5</v>
+        <v>16</v>
       </c>
       <c r="T109"/>
       <c r="U109" t="n">
-        <v>55.9</v>
+        <v>56.4</v>
       </c>
     </row>
     <row r="110">
@@ -6614,38 +6598,54 @@
         <v>2021</v>
       </c>
       <c r="D110" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E110" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F110" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G110" t="n">
-        <v>61</v>
+        <v>3</v>
       </c>
       <c r="H110"/>
       <c r="I110"/>
-      <c r="J110"/>
+      <c r="J110" t="n">
+        <v>16</v>
+      </c>
       <c r="K110" t="s">
-        <v>52</v>
-      </c>
-      <c r="L110"/>
-      <c r="M110"/>
-      <c r="N110"/>
-      <c r="O110"/>
-      <c r="P110"/>
-      <c r="Q110"/>
+        <v>51</v>
+      </c>
+      <c r="L110" t="s">
+        <v>25</v>
+      </c>
+      <c r="M110" t="n">
+        <v>36</v>
+      </c>
+      <c r="N110" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="O110" t="n">
+        <v>19.16</v>
+      </c>
+      <c r="P110" t="n">
+        <v>48.22</v>
+      </c>
+      <c r="Q110" t="n">
+        <v>67.38</v>
+      </c>
       <c r="R110" t="n">
-        <v>2023.9</v>
+        <v>1734.3</v>
       </c>
       <c r="S110" t="n">
-        <v>16</v>
-      </c>
-      <c r="T110"/>
+        <v>13.9</v>
+      </c>
+      <c r="T110" t="n">
+        <v>1.5</v>
+      </c>
       <c r="U110" t="n">
-        <v>56.4</v>
+        <v>56.7</v>
       </c>
     </row>
     <row r="111">
@@ -6665,15 +6665,15 @@
         <v>8</v>
       </c>
       <c r="F111" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G111" t="n">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="H111"/>
       <c r="I111"/>
       <c r="J111" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="K111" t="s">
         <v>51</v>
@@ -6682,31 +6682,31 @@
         <v>25</v>
       </c>
       <c r="M111" t="n">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="N111" t="n">
         <v>1.5</v>
       </c>
       <c r="O111" t="n">
-        <v>19.16</v>
+        <v>18.86</v>
       </c>
       <c r="P111" t="n">
-        <v>48.22</v>
+        <v>50.07</v>
       </c>
       <c r="Q111" t="n">
-        <v>67.38</v>
+        <v>68.93</v>
       </c>
       <c r="R111" t="n">
-        <v>1734.3</v>
+        <v>2225.5</v>
       </c>
       <c r="S111" t="n">
-        <v>13.9</v>
+        <v>14.7</v>
       </c>
       <c r="T111" t="n">
         <v>1.5</v>
       </c>
       <c r="U111" t="n">
-        <v>56.7</v>
+        <v>55.5</v>
       </c>
     </row>
     <row r="112">
@@ -6726,48 +6726,38 @@
         <v>8</v>
       </c>
       <c r="F112" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G112" t="n">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="H112"/>
       <c r="I112"/>
-      <c r="J112" t="n">
-        <v>18</v>
-      </c>
+      <c r="J112"/>
       <c r="K112" t="s">
         <v>51</v>
       </c>
-      <c r="L112" t="s">
-        <v>25</v>
-      </c>
-      <c r="M112" t="n">
-        <v>33</v>
-      </c>
-      <c r="N112" t="n">
-        <v>1.5</v>
-      </c>
+      <c r="L112"/>
+      <c r="M112"/>
+      <c r="N112"/>
       <c r="O112" t="n">
-        <v>18.86</v>
+        <v>18.65</v>
       </c>
       <c r="P112" t="n">
-        <v>50.07</v>
+        <v>48.69</v>
       </c>
       <c r="Q112" t="n">
-        <v>68.93</v>
+        <v>67.34</v>
       </c>
       <c r="R112" t="n">
-        <v>2225.5</v>
+        <v>1861.2</v>
       </c>
       <c r="S112" t="n">
-        <v>14.7</v>
-      </c>
-      <c r="T112" t="n">
-        <v>1.5</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="T112"/>
       <c r="U112" t="n">
-        <v>55.5</v>
+        <v>56.4</v>
       </c>
     </row>
     <row r="113">
@@ -6787,10 +6777,10 @@
         <v>8</v>
       </c>
       <c r="F113" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G113" t="n">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="H113"/>
       <c r="I113"/>
@@ -6801,24 +6791,18 @@
       <c r="L113"/>
       <c r="M113"/>
       <c r="N113"/>
-      <c r="O113" t="n">
-        <v>18.65</v>
-      </c>
-      <c r="P113" t="n">
-        <v>48.69</v>
-      </c>
-      <c r="Q113" t="n">
-        <v>67.34</v>
-      </c>
+      <c r="O113"/>
+      <c r="P113"/>
+      <c r="Q113"/>
       <c r="R113" t="n">
-        <v>1861.2</v>
+        <v>1728.6</v>
       </c>
       <c r="S113" t="n">
         <v>13</v>
       </c>
       <c r="T113"/>
       <c r="U113" t="n">
-        <v>56.4</v>
+        <v>56.6</v>
       </c>
     </row>
     <row r="114">
@@ -6832,38 +6816,54 @@
         <v>2021</v>
       </c>
       <c r="D114" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E114" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F114" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G114" t="n">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="H114"/>
       <c r="I114"/>
-      <c r="J114"/>
+      <c r="J114" t="n">
+        <v>23</v>
+      </c>
       <c r="K114" t="s">
-        <v>51</v>
-      </c>
-      <c r="L114"/>
-      <c r="M114"/>
-      <c r="N114"/>
-      <c r="O114"/>
-      <c r="P114"/>
-      <c r="Q114"/>
+        <v>52</v>
+      </c>
+      <c r="L114" t="s">
+        <v>28</v>
+      </c>
+      <c r="M114" t="n">
+        <v>63</v>
+      </c>
+      <c r="N114" t="n">
+        <v>2</v>
+      </c>
+      <c r="O114" t="n">
+        <v>23.2</v>
+      </c>
+      <c r="P114" t="n">
+        <v>42.29</v>
+      </c>
+      <c r="Q114" t="n">
+        <v>65.49</v>
+      </c>
       <c r="R114" t="n">
-        <v>1728.6</v>
+        <v>1686.4</v>
       </c>
       <c r="S114" t="n">
-        <v>13</v>
-      </c>
-      <c r="T114"/>
+        <v>16.2</v>
+      </c>
+      <c r="T114" t="n">
+        <v>1.5</v>
+      </c>
       <c r="U114" t="n">
-        <v>56.6</v>
+        <v>55</v>
       </c>
     </row>
     <row r="115">
@@ -6883,15 +6883,15 @@
         <v>9</v>
       </c>
       <c r="F115" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G115" t="n">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="H115"/>
       <c r="I115"/>
       <c r="J115" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K115" t="s">
         <v>52</v>
@@ -6900,31 +6900,31 @@
         <v>28</v>
       </c>
       <c r="M115" t="n">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="N115" t="n">
         <v>2</v>
       </c>
       <c r="O115" t="n">
-        <v>23.2</v>
+        <v>22.43</v>
       </c>
       <c r="P115" t="n">
-        <v>42.29</v>
+        <v>43.08</v>
       </c>
       <c r="Q115" t="n">
-        <v>65.49</v>
+        <v>65.51</v>
       </c>
       <c r="R115" t="n">
-        <v>1686.4</v>
+        <v>2202.5</v>
       </c>
       <c r="S115" t="n">
-        <v>16.2</v>
+        <v>15.6</v>
       </c>
       <c r="T115" t="n">
         <v>1.5</v>
       </c>
       <c r="U115" t="n">
-        <v>55</v>
+        <v>54.9</v>
       </c>
     </row>
     <row r="116">
@@ -6944,48 +6944,38 @@
         <v>9</v>
       </c>
       <c r="F116" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G116" t="n">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="H116"/>
       <c r="I116"/>
-      <c r="J116" t="n">
-        <v>21</v>
-      </c>
+      <c r="J116"/>
       <c r="K116" t="s">
         <v>52</v>
       </c>
-      <c r="L116" t="s">
-        <v>28</v>
-      </c>
-      <c r="M116" t="n">
-        <v>60</v>
-      </c>
-      <c r="N116" t="n">
-        <v>2</v>
-      </c>
+      <c r="L116"/>
+      <c r="M116"/>
+      <c r="N116"/>
       <c r="O116" t="n">
-        <v>22.43</v>
+        <v>22.33</v>
       </c>
       <c r="P116" t="n">
-        <v>43.08</v>
+        <v>43.57</v>
       </c>
       <c r="Q116" t="n">
-        <v>65.51</v>
+        <v>65.9</v>
       </c>
       <c r="R116" t="n">
-        <v>2202.5</v>
+        <v>2063.4</v>
       </c>
       <c r="S116" t="n">
-        <v>15.6</v>
-      </c>
-      <c r="T116" t="n">
-        <v>1.5</v>
-      </c>
+        <v>16.4</v>
+      </c>
+      <c r="T116"/>
       <c r="U116" t="n">
-        <v>54.9</v>
+        <v>56</v>
       </c>
     </row>
     <row r="117">
@@ -7005,10 +6995,10 @@
         <v>9</v>
       </c>
       <c r="F117" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G117" t="n">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="H117"/>
       <c r="I117"/>
@@ -7019,24 +7009,18 @@
       <c r="L117"/>
       <c r="M117"/>
       <c r="N117"/>
-      <c r="O117" t="n">
-        <v>22.33</v>
-      </c>
-      <c r="P117" t="n">
-        <v>43.57</v>
-      </c>
-      <c r="Q117" t="n">
-        <v>65.9</v>
-      </c>
+      <c r="O117"/>
+      <c r="P117"/>
+      <c r="Q117"/>
       <c r="R117" t="n">
-        <v>2063.4</v>
+        <v>2196.4</v>
       </c>
       <c r="S117" t="n">
-        <v>16.4</v>
+        <v>15.9</v>
       </c>
       <c r="T117"/>
       <c r="U117" t="n">
-        <v>56</v>
+        <v>55.8</v>
       </c>
     </row>
     <row r="118">
@@ -7050,38 +7034,54 @@
         <v>2021</v>
       </c>
       <c r="D118" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E118" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F118" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G118" t="n">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="H118"/>
       <c r="I118"/>
-      <c r="J118"/>
+      <c r="J118" t="n">
+        <v>25</v>
+      </c>
       <c r="K118" t="s">
         <v>52</v>
       </c>
-      <c r="L118"/>
-      <c r="M118"/>
-      <c r="N118"/>
-      <c r="O118"/>
-      <c r="P118"/>
-      <c r="Q118"/>
+      <c r="L118" t="s">
+        <v>25</v>
+      </c>
+      <c r="M118" t="n">
+        <v>54</v>
+      </c>
+      <c r="N118" t="n">
+        <v>2</v>
+      </c>
+      <c r="O118" t="n">
+        <v>21.62</v>
+      </c>
+      <c r="P118" t="n">
+        <v>43.82</v>
+      </c>
+      <c r="Q118" t="n">
+        <v>65.44</v>
+      </c>
       <c r="R118" t="n">
-        <v>2196.4</v>
+        <v>1236.4</v>
       </c>
       <c r="S118" t="n">
-        <v>15.9</v>
-      </c>
-      <c r="T118"/>
+        <v>16.9</v>
+      </c>
+      <c r="T118" t="n">
+        <v>1.5</v>
+      </c>
       <c r="U118" t="n">
-        <v>55.8</v>
+        <v>57.8</v>
       </c>
     </row>
     <row r="119">
@@ -7101,15 +7101,15 @@
         <v>10</v>
       </c>
       <c r="F119" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G119" t="n">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="H119"/>
       <c r="I119"/>
       <c r="J119" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K119" t="s">
         <v>52</v>
@@ -7118,31 +7118,31 @@
         <v>25</v>
       </c>
       <c r="M119" t="n">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="N119" t="n">
         <v>2</v>
       </c>
       <c r="O119" t="n">
-        <v>21.62</v>
+        <v>21.31</v>
       </c>
       <c r="P119" t="n">
-        <v>43.82</v>
+        <v>44.88</v>
       </c>
       <c r="Q119" t="n">
-        <v>65.44</v>
+        <v>66.19</v>
       </c>
       <c r="R119" t="n">
-        <v>1236.4</v>
+        <v>1602.2</v>
       </c>
       <c r="S119" t="n">
-        <v>16.9</v>
+        <v>17.2</v>
       </c>
       <c r="T119" t="n">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="U119" t="n">
-        <v>57.8</v>
+        <v>56.3</v>
       </c>
     </row>
     <row r="120">
@@ -7162,46 +7162,36 @@
         <v>10</v>
       </c>
       <c r="F120" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G120" t="n">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="H120"/>
       <c r="I120"/>
-      <c r="J120" t="n">
-        <v>23</v>
-      </c>
+      <c r="J120"/>
       <c r="K120" t="s">
         <v>52</v>
       </c>
-      <c r="L120" t="s">
-        <v>25</v>
-      </c>
-      <c r="M120" t="n">
-        <v>57</v>
-      </c>
-      <c r="N120" t="n">
-        <v>2</v>
-      </c>
+      <c r="L120"/>
+      <c r="M120"/>
+      <c r="N120"/>
       <c r="O120" t="n">
-        <v>21.31</v>
+        <v>21.78</v>
       </c>
       <c r="P120" t="n">
-        <v>44.88</v>
+        <v>45.05</v>
       </c>
       <c r="Q120" t="n">
-        <v>66.19</v>
+        <v>66.83</v>
       </c>
       <c r="R120" t="n">
-        <v>1602.2</v>
+        <v>1479.5</v>
       </c>
       <c r="S120" t="n">
-        <v>17.2</v>
-      </c>
-      <c r="T120" t="n">
-        <v>2.5</v>
-      </c>
+        <v>17.4</v>
+      </c>
+      <c r="T120"/>
       <c r="U120" t="n">
         <v>56.3</v>
       </c>
@@ -7223,10 +7213,10 @@
         <v>10</v>
       </c>
       <c r="F121" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G121" t="n">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="H121"/>
       <c r="I121"/>
@@ -7237,24 +7227,18 @@
       <c r="L121"/>
       <c r="M121"/>
       <c r="N121"/>
-      <c r="O121" t="n">
-        <v>21.78</v>
-      </c>
-      <c r="P121" t="n">
-        <v>45.05</v>
-      </c>
-      <c r="Q121" t="n">
-        <v>66.83</v>
-      </c>
+      <c r="O121"/>
+      <c r="P121"/>
+      <c r="Q121"/>
       <c r="R121" t="n">
-        <v>1479.5</v>
+        <v>1159.9</v>
       </c>
       <c r="S121" t="n">
-        <v>17.4</v>
+        <v>15.6</v>
       </c>
       <c r="T121"/>
       <c r="U121" t="n">
-        <v>56.3</v>
+        <v>56.7</v>
       </c>
     </row>
     <row r="122">
@@ -7268,38 +7252,54 @@
         <v>2021</v>
       </c>
       <c r="D122" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E122" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F122" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G122" t="n">
-        <v>71</v>
+        <v>13</v>
       </c>
       <c r="H122"/>
       <c r="I122"/>
-      <c r="J122"/>
+      <c r="J122" t="n">
+        <v>26</v>
+      </c>
       <c r="K122" t="s">
-        <v>52</v>
-      </c>
-      <c r="L122"/>
-      <c r="M122"/>
-      <c r="N122"/>
-      <c r="O122"/>
-      <c r="P122"/>
-      <c r="Q122"/>
+        <v>51</v>
+      </c>
+      <c r="L122" t="s">
+        <v>25</v>
+      </c>
+      <c r="M122" t="n">
+        <v>44</v>
+      </c>
+      <c r="N122" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="O122" t="n">
+        <v>20.42</v>
+      </c>
+      <c r="P122" t="n">
+        <v>44.07</v>
+      </c>
+      <c r="Q122" t="n">
+        <v>64.49</v>
+      </c>
       <c r="R122" t="n">
-        <v>1159.9</v>
+        <v>2205.1</v>
       </c>
       <c r="S122" t="n">
-        <v>15.6</v>
-      </c>
-      <c r="T122"/>
+        <v>13.1</v>
+      </c>
+      <c r="T122" t="n">
+        <v>1.5</v>
+      </c>
       <c r="U122" t="n">
-        <v>56.7</v>
+        <v>58.1</v>
       </c>
     </row>
     <row r="123">
@@ -7319,10 +7319,10 @@
         <v>11</v>
       </c>
       <c r="F123" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G123" t="n">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="H123"/>
       <c r="I123"/>
@@ -7336,31 +7336,31 @@
         <v>25</v>
       </c>
       <c r="M123" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="N123" t="n">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="O123" t="n">
-        <v>20.42</v>
+        <v>20.45</v>
       </c>
       <c r="P123" t="n">
-        <v>44.07</v>
+        <v>44.71</v>
       </c>
       <c r="Q123" t="n">
-        <v>64.49</v>
+        <v>65.16</v>
       </c>
       <c r="R123" t="n">
-        <v>2205.1</v>
+        <v>1819.5</v>
       </c>
       <c r="S123" t="n">
-        <v>13.1</v>
+        <v>12.1</v>
       </c>
       <c r="T123" t="n">
         <v>1.5</v>
       </c>
       <c r="U123" t="n">
-        <v>58.1</v>
+        <v>57.7</v>
       </c>
     </row>
     <row r="124">
@@ -7380,48 +7380,38 @@
         <v>11</v>
       </c>
       <c r="F124" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G124" t="n">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="H124"/>
       <c r="I124"/>
-      <c r="J124" t="n">
-        <v>26</v>
-      </c>
+      <c r="J124"/>
       <c r="K124" t="s">
         <v>51</v>
       </c>
-      <c r="L124" t="s">
-        <v>25</v>
-      </c>
-      <c r="M124" t="n">
-        <v>47</v>
-      </c>
-      <c r="N124" t="n">
-        <v>1</v>
-      </c>
+      <c r="L124"/>
+      <c r="M124"/>
+      <c r="N124"/>
       <c r="O124" t="n">
-        <v>20.45</v>
+        <v>20.42</v>
       </c>
       <c r="P124" t="n">
-        <v>44.71</v>
+        <v>44.32</v>
       </c>
       <c r="Q124" t="n">
-        <v>65.16</v>
+        <v>64.74</v>
       </c>
       <c r="R124" t="n">
-        <v>1819.5</v>
+        <v>2006.8</v>
       </c>
       <c r="S124" t="n">
-        <v>12.1</v>
-      </c>
-      <c r="T124" t="n">
-        <v>1.5</v>
-      </c>
+        <v>13.9</v>
+      </c>
+      <c r="T124"/>
       <c r="U124" t="n">
-        <v>57.7</v>
+        <v>58.1</v>
       </c>
     </row>
     <row r="125">
@@ -7441,10 +7431,10 @@
         <v>11</v>
       </c>
       <c r="F125" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G125" t="n">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="H125"/>
       <c r="I125"/>
@@ -7455,25 +7445,17 @@
       <c r="L125"/>
       <c r="M125"/>
       <c r="N125"/>
-      <c r="O125" t="n">
-        <v>20.42</v>
-      </c>
-      <c r="P125" t="n">
-        <v>44.32</v>
-      </c>
-      <c r="Q125" t="n">
-        <v>64.74</v>
-      </c>
+      <c r="O125"/>
+      <c r="P125"/>
+      <c r="Q125"/>
       <c r="R125" t="n">
-        <v>2006.8</v>
+        <v>1634.6</v>
       </c>
       <c r="S125" t="n">
-        <v>13.9</v>
+        <v>12.8</v>
       </c>
       <c r="T125"/>
-      <c r="U125" t="n">
-        <v>58.1</v>
-      </c>
+      <c r="U125"/>
     </row>
     <row r="126">
       <c r="A126" t="s">
@@ -7486,36 +7468,54 @@
         <v>2021</v>
       </c>
       <c r="D126" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E126" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F126" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G126" t="n">
-        <v>68</v>
+        <v>18</v>
       </c>
       <c r="H126"/>
-      <c r="I126"/>
-      <c r="J126"/>
+      <c r="I126" t="s">
+        <v>54</v>
+      </c>
+      <c r="J126" t="n">
+        <v>22</v>
+      </c>
       <c r="K126" t="s">
-        <v>51</v>
-      </c>
-      <c r="L126"/>
-      <c r="M126"/>
-      <c r="N126"/>
-      <c r="O126"/>
-      <c r="P126"/>
-      <c r="Q126"/>
+        <v>53</v>
+      </c>
+      <c r="L126" t="s">
+        <v>28</v>
+      </c>
+      <c r="M126" t="n">
+        <v>31</v>
+      </c>
+      <c r="N126" t="n">
+        <v>2</v>
+      </c>
+      <c r="O126" t="n">
+        <v>19.66</v>
+      </c>
+      <c r="P126" t="n">
+        <v>47.36</v>
+      </c>
+      <c r="Q126" t="n">
+        <v>67.02</v>
+      </c>
       <c r="R126" t="n">
-        <v>1634.6</v>
+        <v>929.4</v>
       </c>
       <c r="S126" t="n">
-        <v>12.8</v>
-      </c>
-      <c r="T126"/>
+        <v>5.2</v>
+      </c>
+      <c r="T126" t="n">
+        <v>2</v>
+      </c>
       <c r="U126"/>
     </row>
     <row r="127">
@@ -7535,17 +7535,17 @@
         <v>12</v>
       </c>
       <c r="F127" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G127" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H127"/>
       <c r="I127" t="s">
         <v>54</v>
       </c>
       <c r="J127" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K127" t="s">
         <v>53</v>
@@ -7557,22 +7557,22 @@
         <v>31</v>
       </c>
       <c r="N127" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="O127" t="n">
-        <v>19.66</v>
+        <v>18.74</v>
       </c>
       <c r="P127" t="n">
-        <v>47.36</v>
+        <v>44.51</v>
       </c>
       <c r="Q127" t="n">
-        <v>67.02</v>
+        <v>63.25</v>
       </c>
       <c r="R127" t="n">
-        <v>929.4</v>
+        <v>1006.5</v>
       </c>
       <c r="S127" t="n">
-        <v>5.2</v>
+        <v>5.5</v>
       </c>
       <c r="T127" t="n">
         <v>2</v>
@@ -7596,48 +7596,38 @@
         <v>12</v>
       </c>
       <c r="F128" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G128" t="n">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="H128"/>
       <c r="I128" t="s">
         <v>54</v>
       </c>
-      <c r="J128" t="n">
-        <v>21</v>
-      </c>
+      <c r="J128"/>
       <c r="K128" t="s">
         <v>53</v>
       </c>
-      <c r="L128" t="s">
-        <v>28</v>
-      </c>
-      <c r="M128" t="n">
-        <v>31</v>
-      </c>
-      <c r="N128" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="L128"/>
+      <c r="M128"/>
+      <c r="N128"/>
       <c r="O128" t="n">
-        <v>18.74</v>
+        <v>19.83</v>
       </c>
       <c r="P128" t="n">
-        <v>44.51</v>
+        <v>48.01</v>
       </c>
       <c r="Q128" t="n">
-        <v>63.25</v>
+        <v>67.84</v>
       </c>
       <c r="R128" t="n">
-        <v>1006.5</v>
+        <v>1185.1</v>
       </c>
       <c r="S128" t="n">
-        <v>5.5</v>
-      </c>
-      <c r="T128" t="n">
-        <v>2</v>
-      </c>
+        <v>6.5</v>
+      </c>
+      <c r="T128"/>
       <c r="U128"/>
     </row>
     <row r="129">
@@ -7657,10 +7647,10 @@
         <v>12</v>
       </c>
       <c r="F129" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G129" t="n">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="H129"/>
       <c r="I129" t="s">
@@ -7673,20 +7663,14 @@
       <c r="L129"/>
       <c r="M129"/>
       <c r="N129"/>
-      <c r="O129" t="n">
-        <v>19.83</v>
-      </c>
-      <c r="P129" t="n">
-        <v>48.01</v>
-      </c>
-      <c r="Q129" t="n">
-        <v>67.84</v>
-      </c>
+      <c r="O129"/>
+      <c r="P129"/>
+      <c r="Q129"/>
       <c r="R129" t="n">
-        <v>1185.1</v>
+        <v>659.8</v>
       </c>
       <c r="S129" t="n">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="T129"/>
       <c r="U129"/>
@@ -7702,38 +7686,52 @@
         <v>2021</v>
       </c>
       <c r="D130" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E130" t="n">
+        <v>13</v>
+      </c>
+      <c r="F130" t="n">
+        <v>1</v>
+      </c>
+      <c r="G130" t="n">
+        <v>5</v>
+      </c>
+      <c r="H130"/>
+      <c r="I130"/>
+      <c r="J130" t="n">
         <v>12</v>
       </c>
-      <c r="F130" t="n">
-        <v>4</v>
-      </c>
-      <c r="G130" t="n">
-        <v>69</v>
-      </c>
-      <c r="H130"/>
-      <c r="I130" t="s">
-        <v>54</v>
-      </c>
-      <c r="J130"/>
       <c r="K130" t="s">
-        <v>53</v>
-      </c>
-      <c r="L130"/>
-      <c r="M130"/>
-      <c r="N130"/>
-      <c r="O130"/>
-      <c r="P130"/>
-      <c r="Q130"/>
+        <v>52</v>
+      </c>
+      <c r="L130" t="s">
+        <v>25</v>
+      </c>
+      <c r="M130" t="n">
+        <v>29</v>
+      </c>
+      <c r="N130" t="n">
+        <v>1</v>
+      </c>
+      <c r="O130" t="n">
+        <v>18.38</v>
+      </c>
+      <c r="P130" t="n">
+        <v>50.38</v>
+      </c>
+      <c r="Q130" t="n">
+        <v>68.76</v>
+      </c>
       <c r="R130" t="n">
-        <v>659.8</v>
+        <v>1774.7</v>
       </c>
       <c r="S130" t="n">
-        <v>6.4</v>
-      </c>
-      <c r="T130"/>
+        <v>15.3</v>
+      </c>
+      <c r="T130" t="n">
+        <v>1.5</v>
+      </c>
       <c r="U130"/>
     </row>
     <row r="131">
@@ -7753,15 +7751,15 @@
         <v>13</v>
       </c>
       <c r="F131" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G131" t="n">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="H131"/>
       <c r="I131"/>
       <c r="J131" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K131" t="s">
         <v>52</v>
@@ -7770,25 +7768,25 @@
         <v>25</v>
       </c>
       <c r="M131" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N131" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="O131" t="n">
-        <v>18.38</v>
+        <v>18.22</v>
       </c>
       <c r="P131" t="n">
-        <v>50.38</v>
+        <v>51.44</v>
       </c>
       <c r="Q131" t="n">
-        <v>68.76</v>
+        <v>69.66</v>
       </c>
       <c r="R131" t="n">
-        <v>1774.7</v>
+        <v>1766.9</v>
       </c>
       <c r="S131" t="n">
-        <v>15.3</v>
+        <v>16.9</v>
       </c>
       <c r="T131" t="n">
         <v>1.5</v>
@@ -7812,46 +7810,36 @@
         <v>13</v>
       </c>
       <c r="F132" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G132" t="n">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="H132"/>
       <c r="I132"/>
-      <c r="J132" t="n">
-        <v>13</v>
-      </c>
+      <c r="J132"/>
       <c r="K132" t="s">
         <v>52</v>
       </c>
-      <c r="L132" t="s">
-        <v>25</v>
-      </c>
-      <c r="M132" t="n">
-        <v>30</v>
-      </c>
-      <c r="N132" t="n">
-        <v>1.5</v>
-      </c>
+      <c r="L132"/>
+      <c r="M132"/>
+      <c r="N132"/>
       <c r="O132" t="n">
-        <v>18.22</v>
+        <v>18.08</v>
       </c>
       <c r="P132" t="n">
-        <v>51.44</v>
+        <v>51.99</v>
       </c>
       <c r="Q132" t="n">
-        <v>69.66</v>
+        <v>70.07</v>
       </c>
       <c r="R132" t="n">
-        <v>1766.9</v>
+        <v>1912.9</v>
       </c>
       <c r="S132" t="n">
-        <v>16.9</v>
-      </c>
-      <c r="T132" t="n">
-        <v>1.5</v>
-      </c>
+        <v>15.5</v>
+      </c>
+      <c r="T132"/>
       <c r="U132"/>
     </row>
     <row r="133">
@@ -7871,10 +7859,10 @@
         <v>13</v>
       </c>
       <c r="F133" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G133" t="n">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="H133"/>
       <c r="I133"/>
@@ -7885,20 +7873,14 @@
       <c r="L133"/>
       <c r="M133"/>
       <c r="N133"/>
-      <c r="O133" t="n">
-        <v>18.08</v>
-      </c>
-      <c r="P133" t="n">
-        <v>51.99</v>
-      </c>
-      <c r="Q133" t="n">
-        <v>70.07</v>
-      </c>
+      <c r="O133"/>
+      <c r="P133"/>
+      <c r="Q133"/>
       <c r="R133" t="n">
-        <v>1912.9</v>
+        <v>1720.8</v>
       </c>
       <c r="S133" t="n">
-        <v>15.5</v>
+        <v>14.8</v>
       </c>
       <c r="T133"/>
       <c r="U133"/>
@@ -7914,36 +7896,52 @@
         <v>2021</v>
       </c>
       <c r="D134" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E134" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F134" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G134" t="n">
-        <v>76</v>
+        <v>9</v>
       </c>
       <c r="H134"/>
       <c r="I134"/>
-      <c r="J134"/>
+      <c r="J134" t="n">
+        <v>18</v>
+      </c>
       <c r="K134" t="s">
         <v>52</v>
       </c>
-      <c r="L134"/>
-      <c r="M134"/>
-      <c r="N134"/>
-      <c r="O134"/>
-      <c r="P134"/>
-      <c r="Q134"/>
+      <c r="L134" t="s">
+        <v>25</v>
+      </c>
+      <c r="M134" t="n">
+        <v>41</v>
+      </c>
+      <c r="N134" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="O134" t="n">
+        <v>19.94</v>
+      </c>
+      <c r="P134" t="n">
+        <v>46.97</v>
+      </c>
+      <c r="Q134" t="n">
+        <v>66.91</v>
+      </c>
       <c r="R134" t="n">
-        <v>1720.8</v>
+        <v>1412.9</v>
       </c>
       <c r="S134" t="n">
-        <v>14.8</v>
-      </c>
-      <c r="T134"/>
+        <v>9.9</v>
+      </c>
+      <c r="T134" t="n">
+        <v>1.5</v>
+      </c>
       <c r="U134"/>
     </row>
     <row r="135">
@@ -7963,15 +7961,15 @@
         <v>14</v>
       </c>
       <c r="F135" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G135" t="n">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="H135"/>
       <c r="I135"/>
       <c r="J135" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K135" t="s">
         <v>52</v>
@@ -7980,25 +7978,25 @@
         <v>25</v>
       </c>
       <c r="M135" t="n">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N135" t="n">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="O135" t="n">
-        <v>19.94</v>
+        <v>19.72</v>
       </c>
       <c r="P135" t="n">
-        <v>46.97</v>
+        <v>46.88</v>
       </c>
       <c r="Q135" t="n">
-        <v>66.91</v>
+        <v>66.6</v>
       </c>
       <c r="R135" t="n">
-        <v>1412.9</v>
+        <v>2009.2</v>
       </c>
       <c r="S135" t="n">
-        <v>9.9</v>
+        <v>11.2</v>
       </c>
       <c r="T135" t="n">
         <v>1.5</v>
@@ -8022,46 +8020,36 @@
         <v>14</v>
       </c>
       <c r="F136" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G136" t="n">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="H136"/>
       <c r="I136"/>
-      <c r="J136" t="n">
-        <v>19</v>
-      </c>
+      <c r="J136"/>
       <c r="K136" t="s">
         <v>52</v>
       </c>
-      <c r="L136" t="s">
-        <v>25</v>
-      </c>
-      <c r="M136" t="n">
-        <v>39</v>
-      </c>
-      <c r="N136" t="n">
-        <v>2</v>
-      </c>
+      <c r="L136"/>
+      <c r="M136"/>
+      <c r="N136"/>
       <c r="O136" t="n">
-        <v>19.72</v>
+        <v>20.44</v>
       </c>
       <c r="P136" t="n">
-        <v>46.88</v>
+        <v>46.4</v>
       </c>
       <c r="Q136" t="n">
-        <v>66.6</v>
+        <v>66.84</v>
       </c>
       <c r="R136" t="n">
-        <v>2009.2</v>
+        <v>2009.4</v>
       </c>
       <c r="S136" t="n">
-        <v>11.2</v>
-      </c>
-      <c r="T136" t="n">
-        <v>1.5</v>
-      </c>
+        <v>12.1</v>
+      </c>
+      <c r="T136"/>
       <c r="U136"/>
     </row>
     <row r="137">
@@ -8081,10 +8069,10 @@
         <v>14</v>
       </c>
       <c r="F137" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G137" t="n">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="H137"/>
       <c r="I137"/>
@@ -8095,20 +8083,14 @@
       <c r="L137"/>
       <c r="M137"/>
       <c r="N137"/>
-      <c r="O137" t="n">
-        <v>20.44</v>
-      </c>
-      <c r="P137" t="n">
-        <v>46.4</v>
-      </c>
-      <c r="Q137" t="n">
-        <v>66.84</v>
-      </c>
+      <c r="O137"/>
+      <c r="P137"/>
+      <c r="Q137"/>
       <c r="R137" t="n">
-        <v>2009.4</v>
+        <v>1732</v>
       </c>
       <c r="S137" t="n">
-        <v>12.1</v>
+        <v>11.2</v>
       </c>
       <c r="T137"/>
       <c r="U137"/>
@@ -8124,36 +8106,52 @@
         <v>2021</v>
       </c>
       <c r="D138" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E138" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F138" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G138" t="n">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="H138"/>
       <c r="I138"/>
-      <c r="J138"/>
+      <c r="J138" t="n">
+        <v>17</v>
+      </c>
       <c r="K138" t="s">
-        <v>52</v>
-      </c>
-      <c r="L138"/>
-      <c r="M138"/>
-      <c r="N138"/>
-      <c r="O138"/>
-      <c r="P138"/>
-      <c r="Q138"/>
+        <v>51</v>
+      </c>
+      <c r="L138" t="s">
+        <v>25</v>
+      </c>
+      <c r="M138" t="n">
+        <v>36</v>
+      </c>
+      <c r="N138" t="n">
+        <v>2</v>
+      </c>
+      <c r="O138" t="n">
+        <v>18.72</v>
+      </c>
+      <c r="P138" t="n">
+        <v>48.89</v>
+      </c>
+      <c r="Q138" t="n">
+        <v>67.61</v>
+      </c>
       <c r="R138" t="n">
-        <v>1732</v>
+        <v>1864.6</v>
       </c>
       <c r="S138" t="n">
-        <v>11.2</v>
-      </c>
-      <c r="T138"/>
+        <v>15</v>
+      </c>
+      <c r="T138" t="n">
+        <v>1.5</v>
+      </c>
       <c r="U138"/>
     </row>
     <row r="139">
@@ -8173,15 +8171,15 @@
         <v>15</v>
       </c>
       <c r="F139" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G139" t="n">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="H139"/>
       <c r="I139"/>
       <c r="J139" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K139" t="s">
         <v>51</v>
@@ -8190,25 +8188,25 @@
         <v>25</v>
       </c>
       <c r="M139" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N139" t="n">
         <v>2</v>
       </c>
       <c r="O139" t="n">
-        <v>18.72</v>
+        <v>18.54</v>
       </c>
       <c r="P139" t="n">
-        <v>48.89</v>
+        <v>49.55</v>
       </c>
       <c r="Q139" t="n">
-        <v>67.61</v>
+        <v>68.09</v>
       </c>
       <c r="R139" t="n">
-        <v>1864.6</v>
+        <v>2073.8</v>
       </c>
       <c r="S139" t="n">
-        <v>15</v>
+        <v>14.5</v>
       </c>
       <c r="T139" t="n">
         <v>1.5</v>
@@ -8232,46 +8230,36 @@
         <v>15</v>
       </c>
       <c r="F140" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G140" t="n">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="H140"/>
       <c r="I140"/>
-      <c r="J140" t="n">
-        <v>18</v>
-      </c>
+      <c r="J140"/>
       <c r="K140" t="s">
         <v>51</v>
       </c>
-      <c r="L140" t="s">
-        <v>25</v>
-      </c>
-      <c r="M140" t="n">
-        <v>35</v>
-      </c>
-      <c r="N140" t="n">
-        <v>2</v>
-      </c>
+      <c r="L140"/>
+      <c r="M140"/>
+      <c r="N140"/>
       <c r="O140" t="n">
-        <v>18.54</v>
+        <v>18.36</v>
       </c>
       <c r="P140" t="n">
-        <v>49.55</v>
+        <v>48.78</v>
       </c>
       <c r="Q140" t="n">
-        <v>68.09</v>
+        <v>67.14</v>
       </c>
       <c r="R140" t="n">
-        <v>2073.8</v>
+        <v>1683</v>
       </c>
       <c r="S140" t="n">
-        <v>14.5</v>
-      </c>
-      <c r="T140" t="n">
-        <v>1.5</v>
-      </c>
+        <v>13.8</v>
+      </c>
+      <c r="T140"/>
       <c r="U140"/>
     </row>
     <row r="141">
@@ -8291,10 +8279,10 @@
         <v>15</v>
       </c>
       <c r="F141" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G141" t="n">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="H141"/>
       <c r="I141"/>
@@ -8305,20 +8293,14 @@
       <c r="L141"/>
       <c r="M141"/>
       <c r="N141"/>
-      <c r="O141" t="n">
-        <v>18.36</v>
-      </c>
-      <c r="P141" t="n">
-        <v>48.78</v>
-      </c>
-      <c r="Q141" t="n">
-        <v>67.14</v>
-      </c>
+      <c r="O141"/>
+      <c r="P141"/>
+      <c r="Q141"/>
       <c r="R141" t="n">
-        <v>1683</v>
+        <v>2206.1</v>
       </c>
       <c r="S141" t="n">
-        <v>13.8</v>
+        <v>13.9</v>
       </c>
       <c r="T141"/>
       <c r="U141"/>
@@ -8334,36 +8316,52 @@
         <v>2021</v>
       </c>
       <c r="D142" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E142" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F142" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G142" t="n">
-        <v>70</v>
+        <v>8</v>
       </c>
       <c r="H142"/>
       <c r="I142"/>
-      <c r="J142"/>
+      <c r="J142" t="n">
+        <v>20</v>
+      </c>
       <c r="K142" t="s">
-        <v>51</v>
-      </c>
-      <c r="L142"/>
-      <c r="M142"/>
-      <c r="N142"/>
-      <c r="O142"/>
-      <c r="P142"/>
-      <c r="Q142"/>
+        <v>52</v>
+      </c>
+      <c r="L142" t="s">
+        <v>28</v>
+      </c>
+      <c r="M142" t="n">
+        <v>42</v>
+      </c>
+      <c r="N142" t="n">
+        <v>2</v>
+      </c>
+      <c r="O142" t="n">
+        <v>20.31</v>
+      </c>
+      <c r="P142" t="n">
+        <v>46.52</v>
+      </c>
+      <c r="Q142" t="n">
+        <v>66.83</v>
+      </c>
       <c r="R142" t="n">
-        <v>2206.1</v>
+        <v>1794.2</v>
       </c>
       <c r="S142" t="n">
-        <v>13.9</v>
-      </c>
-      <c r="T142"/>
+        <v>13.3</v>
+      </c>
+      <c r="T142" t="n">
+        <v>1.5</v>
+      </c>
       <c r="U142"/>
     </row>
     <row r="143">
@@ -8383,15 +8381,15 @@
         <v>16</v>
       </c>
       <c r="F143" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G143" t="n">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="H143"/>
       <c r="I143"/>
       <c r="J143" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K143" t="s">
         <v>52</v>
@@ -8400,25 +8398,25 @@
         <v>28</v>
       </c>
       <c r="M143" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N143" t="n">
         <v>2</v>
       </c>
       <c r="O143" t="n">
-        <v>20.31</v>
+        <v>19.71</v>
       </c>
       <c r="P143" t="n">
-        <v>46.52</v>
+        <v>47.13</v>
       </c>
       <c r="Q143" t="n">
-        <v>66.83</v>
+        <v>66.84</v>
       </c>
       <c r="R143" t="n">
-        <v>1794.2</v>
+        <v>2102.2</v>
       </c>
       <c r="S143" t="n">
-        <v>13.3</v>
+        <v>13.4</v>
       </c>
       <c r="T143" t="n">
         <v>1.5</v>
@@ -8442,46 +8440,36 @@
         <v>16</v>
       </c>
       <c r="F144" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G144" t="n">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="H144"/>
       <c r="I144"/>
-      <c r="J144" t="n">
-        <v>19</v>
-      </c>
+      <c r="J144"/>
       <c r="K144" t="s">
         <v>52</v>
       </c>
-      <c r="L144" t="s">
-        <v>28</v>
-      </c>
-      <c r="M144" t="n">
-        <v>41</v>
-      </c>
-      <c r="N144" t="n">
-        <v>2</v>
-      </c>
+      <c r="L144"/>
+      <c r="M144"/>
+      <c r="N144"/>
       <c r="O144" t="n">
-        <v>19.71</v>
+        <v>18.92</v>
       </c>
       <c r="P144" t="n">
-        <v>47.13</v>
+        <v>47.79</v>
       </c>
       <c r="Q144" t="n">
-        <v>66.84</v>
+        <v>66.71</v>
       </c>
       <c r="R144" t="n">
-        <v>2102.2</v>
+        <v>1717.6</v>
       </c>
       <c r="S144" t="n">
-        <v>13.4</v>
-      </c>
-      <c r="T144" t="n">
-        <v>1.5</v>
-      </c>
+        <v>13.1</v>
+      </c>
+      <c r="T144"/>
       <c r="U144"/>
     </row>
     <row r="145">
@@ -8501,10 +8489,10 @@
         <v>16</v>
       </c>
       <c r="F145" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G145" t="n">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="H145"/>
       <c r="I145"/>
@@ -8515,20 +8503,14 @@
       <c r="L145"/>
       <c r="M145"/>
       <c r="N145"/>
-      <c r="O145" t="n">
-        <v>18.92</v>
-      </c>
-      <c r="P145" t="n">
-        <v>47.79</v>
-      </c>
-      <c r="Q145" t="n">
-        <v>66.71</v>
-      </c>
+      <c r="O145"/>
+      <c r="P145"/>
+      <c r="Q145"/>
       <c r="R145" t="n">
-        <v>1717.6</v>
+        <v>1773.4</v>
       </c>
       <c r="S145" t="n">
-        <v>13.1</v>
+        <v>13.7</v>
       </c>
       <c r="T145"/>
       <c r="U145"/>
@@ -8544,36 +8526,52 @@
         <v>2021</v>
       </c>
       <c r="D146" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E146" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F146" t="n">
+        <v>1</v>
+      </c>
+      <c r="G146" t="n">
         <v>4</v>
-      </c>
-      <c r="G146" t="n">
-        <v>64</v>
       </c>
       <c r="H146"/>
       <c r="I146"/>
-      <c r="J146"/>
+      <c r="J146" t="n">
+        <v>18</v>
+      </c>
       <c r="K146" t="s">
         <v>52</v>
       </c>
-      <c r="L146"/>
-      <c r="M146"/>
-      <c r="N146"/>
-      <c r="O146"/>
-      <c r="P146"/>
-      <c r="Q146"/>
+      <c r="L146" t="s">
+        <v>28</v>
+      </c>
+      <c r="M146" t="n">
+        <v>30</v>
+      </c>
+      <c r="N146" t="n">
+        <v>1</v>
+      </c>
+      <c r="O146" t="n">
+        <v>22.54</v>
+      </c>
+      <c r="P146" t="n">
+        <v>40.06</v>
+      </c>
+      <c r="Q146" t="n">
+        <v>62.6</v>
+      </c>
       <c r="R146" t="n">
-        <v>1773.4</v>
+        <v>2733.9</v>
       </c>
       <c r="S146" t="n">
         <v>13.7</v>
       </c>
-      <c r="T146"/>
+      <c r="T146" t="n">
+        <v>1.5</v>
+      </c>
       <c r="U146"/>
     </row>
     <row r="147">
@@ -8593,15 +8591,15 @@
         <v>17</v>
       </c>
       <c r="F147" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G147" t="n">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="H147"/>
       <c r="I147"/>
       <c r="J147" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K147" t="s">
         <v>52</v>
@@ -8610,25 +8608,23 @@
         <v>28</v>
       </c>
       <c r="M147" t="n">
-        <v>30</v>
-      </c>
-      <c r="N147" t="n">
-        <v>1</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="N147"/>
       <c r="O147" t="n">
-        <v>22.54</v>
+        <v>21.59</v>
       </c>
       <c r="P147" t="n">
-        <v>40.06</v>
+        <v>40.91</v>
       </c>
       <c r="Q147" t="n">
-        <v>62.6</v>
+        <v>62.5</v>
       </c>
       <c r="R147" t="n">
-        <v>2733.9</v>
+        <v>2557.8</v>
       </c>
       <c r="S147" t="n">
-        <v>13.7</v>
+        <v>13.9</v>
       </c>
       <c r="T147" t="n">
         <v>1.5</v>
@@ -8652,44 +8648,36 @@
         <v>17</v>
       </c>
       <c r="F148" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G148" t="n">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="H148"/>
       <c r="I148"/>
-      <c r="J148" t="n">
-        <v>17</v>
-      </c>
+      <c r="J148"/>
       <c r="K148" t="s">
         <v>52</v>
       </c>
-      <c r="L148" t="s">
-        <v>28</v>
-      </c>
-      <c r="M148" t="n">
-        <v>32</v>
-      </c>
+      <c r="L148"/>
+      <c r="M148"/>
       <c r="N148"/>
       <c r="O148" t="n">
-        <v>21.59</v>
+        <v>22.58</v>
       </c>
       <c r="P148" t="n">
-        <v>40.91</v>
+        <v>40.95</v>
       </c>
       <c r="Q148" t="n">
-        <v>62.5</v>
+        <v>63.53</v>
       </c>
       <c r="R148" t="n">
-        <v>2557.8</v>
+        <v>2715.4</v>
       </c>
       <c r="S148" t="n">
-        <v>13.9</v>
-      </c>
-      <c r="T148" t="n">
-        <v>1.5</v>
-      </c>
+        <v>10.2</v>
+      </c>
+      <c r="T148"/>
       <c r="U148"/>
     </row>
     <row r="149">
@@ -8709,10 +8697,10 @@
         <v>17</v>
       </c>
       <c r="F149" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G149" t="n">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="H149"/>
       <c r="I149"/>
@@ -8723,20 +8711,14 @@
       <c r="L149"/>
       <c r="M149"/>
       <c r="N149"/>
-      <c r="O149" t="n">
-        <v>22.58</v>
-      </c>
-      <c r="P149" t="n">
-        <v>40.95</v>
-      </c>
-      <c r="Q149" t="n">
-        <v>63.53</v>
-      </c>
+      <c r="O149"/>
+      <c r="P149"/>
+      <c r="Q149"/>
       <c r="R149" t="n">
-        <v>2715.4</v>
+        <v>2398</v>
       </c>
       <c r="S149" t="n">
-        <v>10.2</v>
+        <v>14.2</v>
       </c>
       <c r="T149"/>
       <c r="U149"/>
@@ -8752,36 +8734,52 @@
         <v>2021</v>
       </c>
       <c r="D150" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E150" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F150" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G150" t="n">
-        <v>74</v>
+        <v>10</v>
       </c>
       <c r="H150"/>
       <c r="I150"/>
-      <c r="J150"/>
+      <c r="J150" t="n">
+        <v>19</v>
+      </c>
       <c r="K150" t="s">
         <v>52</v>
       </c>
-      <c r="L150"/>
-      <c r="M150"/>
-      <c r="N150"/>
-      <c r="O150"/>
-      <c r="P150"/>
-      <c r="Q150"/>
+      <c r="L150" t="s">
+        <v>28</v>
+      </c>
+      <c r="M150" t="n">
+        <v>29</v>
+      </c>
+      <c r="N150" t="n">
+        <v>1</v>
+      </c>
+      <c r="O150" t="n">
+        <v>22.85</v>
+      </c>
+      <c r="P150" t="n">
+        <v>40.58</v>
+      </c>
+      <c r="Q150" t="n">
+        <v>63.43</v>
+      </c>
       <c r="R150" t="n">
-        <v>2398</v>
+        <v>2426.5</v>
       </c>
       <c r="S150" t="n">
         <v>14.2</v>
       </c>
-      <c r="T150"/>
+      <c r="T150" t="n">
+        <v>2.5</v>
+      </c>
       <c r="U150"/>
     </row>
     <row r="151">
@@ -8801,15 +8799,15 @@
         <v>18</v>
       </c>
       <c r="F151" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G151" t="n">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H151"/>
       <c r="I151"/>
       <c r="J151" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K151" t="s">
         <v>52</v>
@@ -8818,28 +8816,28 @@
         <v>28</v>
       </c>
       <c r="M151" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N151" t="n">
         <v>1</v>
       </c>
       <c r="O151" t="n">
-        <v>22.85</v>
+        <v>23.14</v>
       </c>
       <c r="P151" t="n">
-        <v>40.58</v>
+        <v>41.33</v>
       </c>
       <c r="Q151" t="n">
-        <v>63.43</v>
+        <v>64.47</v>
       </c>
       <c r="R151" t="n">
-        <v>2426.5</v>
+        <v>1784.8</v>
       </c>
       <c r="S151" t="n">
-        <v>14.2</v>
+        <v>17.2</v>
       </c>
       <c r="T151" t="n">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="U151"/>
     </row>
@@ -8860,46 +8858,36 @@
         <v>18</v>
       </c>
       <c r="F152" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G152" t="n">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="H152"/>
       <c r="I152"/>
-      <c r="J152" t="n">
-        <v>18</v>
-      </c>
+      <c r="J152"/>
       <c r="K152" t="s">
         <v>52</v>
       </c>
-      <c r="L152" t="s">
-        <v>28</v>
-      </c>
-      <c r="M152" t="n">
-        <v>30</v>
-      </c>
-      <c r="N152" t="n">
-        <v>1</v>
-      </c>
+      <c r="L152"/>
+      <c r="M152"/>
+      <c r="N152"/>
       <c r="O152" t="n">
-        <v>23.14</v>
+        <v>23.4</v>
       </c>
       <c r="P152" t="n">
-        <v>41.33</v>
+        <v>42.48</v>
       </c>
       <c r="Q152" t="n">
-        <v>64.47</v>
+        <v>65.88</v>
       </c>
       <c r="R152" t="n">
-        <v>1784.8</v>
+        <v>2270</v>
       </c>
       <c r="S152" t="n">
-        <v>17.2</v>
-      </c>
-      <c r="T152" t="n">
-        <v>1.5</v>
-      </c>
+        <v>16.4</v>
+      </c>
+      <c r="T152"/>
       <c r="U152"/>
     </row>
     <row r="153">
@@ -8919,10 +8907,10 @@
         <v>18</v>
       </c>
       <c r="F153" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G153" t="n">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="H153"/>
       <c r="I153"/>
@@ -8933,20 +8921,14 @@
       <c r="L153"/>
       <c r="M153"/>
       <c r="N153"/>
-      <c r="O153" t="n">
-        <v>23.4</v>
-      </c>
-      <c r="P153" t="n">
-        <v>42.48</v>
-      </c>
-      <c r="Q153" t="n">
-        <v>65.88</v>
-      </c>
+      <c r="O153"/>
+      <c r="P153"/>
+      <c r="Q153"/>
       <c r="R153" t="n">
-        <v>2270</v>
+        <v>1776.3</v>
       </c>
       <c r="S153" t="n">
-        <v>16.4</v>
+        <v>14.1</v>
       </c>
       <c r="T153"/>
       <c r="U153"/>
@@ -8962,36 +8944,52 @@
         <v>2021</v>
       </c>
       <c r="D154" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E154" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F154" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G154" t="n">
-        <v>78</v>
+        <v>1</v>
       </c>
       <c r="H154"/>
       <c r="I154"/>
-      <c r="J154"/>
+      <c r="J154" t="n">
+        <v>10</v>
+      </c>
       <c r="K154" t="s">
         <v>52</v>
       </c>
-      <c r="L154"/>
-      <c r="M154"/>
-      <c r="N154"/>
-      <c r="O154"/>
-      <c r="P154"/>
-      <c r="Q154"/>
+      <c r="L154" t="s">
+        <v>25</v>
+      </c>
+      <c r="M154" t="n">
+        <v>32</v>
+      </c>
+      <c r="N154" t="n">
+        <v>1</v>
+      </c>
+      <c r="O154" t="n">
+        <v>20.63</v>
+      </c>
+      <c r="P154" t="n">
+        <v>45.57</v>
+      </c>
+      <c r="Q154" t="n">
+        <v>66.2</v>
+      </c>
       <c r="R154" t="n">
-        <v>1776.3</v>
+        <v>2050.7</v>
       </c>
       <c r="S154" t="n">
-        <v>14.1</v>
-      </c>
-      <c r="T154"/>
+        <v>11.7</v>
+      </c>
+      <c r="T154" t="n">
+        <v>1.5</v>
+      </c>
       <c r="U154"/>
     </row>
     <row r="155">
@@ -9011,15 +9009,15 @@
         <v>19</v>
       </c>
       <c r="F155" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G155" t="n">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="H155"/>
       <c r="I155"/>
       <c r="J155" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="K155" t="s">
         <v>52</v>
@@ -9031,22 +9029,22 @@
         <v>32</v>
       </c>
       <c r="N155" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="O155" t="n">
-        <v>20.63</v>
+        <v>20.56</v>
       </c>
       <c r="P155" t="n">
-        <v>45.57</v>
+        <v>45.84</v>
       </c>
       <c r="Q155" t="n">
-        <v>66.2</v>
+        <v>66.4</v>
       </c>
       <c r="R155" t="n">
-        <v>2050.7</v>
+        <v>2304.5</v>
       </c>
       <c r="S155" t="n">
-        <v>11.7</v>
+        <v>14.4</v>
       </c>
       <c r="T155" t="n">
         <v>1.5</v>
@@ -9070,46 +9068,36 @@
         <v>19</v>
       </c>
       <c r="F156" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G156" t="n">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="H156"/>
       <c r="I156"/>
-      <c r="J156" t="n">
-        <v>13</v>
-      </c>
+      <c r="J156"/>
       <c r="K156" t="s">
         <v>52</v>
       </c>
-      <c r="L156" t="s">
-        <v>25</v>
-      </c>
-      <c r="M156" t="n">
-        <v>32</v>
-      </c>
-      <c r="N156" t="n">
-        <v>1.5</v>
-      </c>
+      <c r="L156"/>
+      <c r="M156"/>
+      <c r="N156"/>
       <c r="O156" t="n">
-        <v>20.56</v>
+        <v>21.44</v>
       </c>
       <c r="P156" t="n">
-        <v>45.84</v>
+        <v>44.36</v>
       </c>
       <c r="Q156" t="n">
-        <v>66.4</v>
+        <v>65.8</v>
       </c>
       <c r="R156" t="n">
-        <v>2304.5</v>
+        <v>2234</v>
       </c>
       <c r="S156" t="n">
-        <v>14.4</v>
-      </c>
-      <c r="T156" t="n">
-        <v>1.5</v>
-      </c>
+        <v>13.9</v>
+      </c>
+      <c r="T156"/>
       <c r="U156"/>
     </row>
     <row r="157">
@@ -9129,10 +9117,10 @@
         <v>19</v>
       </c>
       <c r="F157" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G157" t="n">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="H157"/>
       <c r="I157"/>
@@ -9143,20 +9131,14 @@
       <c r="L157"/>
       <c r="M157"/>
       <c r="N157"/>
-      <c r="O157" t="n">
-        <v>21.44</v>
-      </c>
-      <c r="P157" t="n">
-        <v>44.36</v>
-      </c>
-      <c r="Q157" t="n">
-        <v>65.8</v>
-      </c>
+      <c r="O157"/>
+      <c r="P157"/>
+      <c r="Q157"/>
       <c r="R157" t="n">
-        <v>2234</v>
+        <v>1843.2</v>
       </c>
       <c r="S157" t="n">
-        <v>13.9</v>
+        <v>12.9</v>
       </c>
       <c r="T157"/>
       <c r="U157"/>
@@ -9172,36 +9154,52 @@
         <v>2021</v>
       </c>
       <c r="D158" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E158" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F158" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G158" t="n">
-        <v>80</v>
+        <v>16</v>
       </c>
       <c r="H158"/>
       <c r="I158"/>
-      <c r="J158"/>
+      <c r="J158" t="n">
+        <v>16</v>
+      </c>
       <c r="K158" t="s">
-        <v>52</v>
-      </c>
-      <c r="L158"/>
-      <c r="M158"/>
-      <c r="N158"/>
-      <c r="O158"/>
-      <c r="P158"/>
-      <c r="Q158"/>
+        <v>51</v>
+      </c>
+      <c r="L158" t="s">
+        <v>28</v>
+      </c>
+      <c r="M158" t="n">
+        <v>44</v>
+      </c>
+      <c r="N158" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="O158" t="n">
+        <v>21.79</v>
+      </c>
+      <c r="P158" t="n">
+        <v>43.47</v>
+      </c>
+      <c r="Q158" t="n">
+        <v>65.26</v>
+      </c>
       <c r="R158" t="n">
-        <v>1843.2</v>
+        <v>1934.4</v>
       </c>
       <c r="S158" t="n">
-        <v>12.9</v>
-      </c>
-      <c r="T158"/>
+        <v>13.6</v>
+      </c>
+      <c r="T158" t="n">
+        <v>1.5</v>
+      </c>
       <c r="U158"/>
     </row>
     <row r="159">
@@ -9221,15 +9219,15 @@
         <v>20</v>
       </c>
       <c r="F159" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G159" t="n">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="H159"/>
       <c r="I159"/>
       <c r="J159" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K159" t="s">
         <v>51</v>
@@ -9238,25 +9236,25 @@
         <v>28</v>
       </c>
       <c r="M159" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="N159" t="n">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="O159" t="n">
-        <v>21.79</v>
+        <v>22.22</v>
       </c>
       <c r="P159" t="n">
-        <v>43.47</v>
+        <v>42.84</v>
       </c>
       <c r="Q159" t="n">
-        <v>65.26</v>
+        <v>65.06</v>
       </c>
       <c r="R159" t="n">
-        <v>1934.4</v>
+        <v>1634.5</v>
       </c>
       <c r="S159" t="n">
-        <v>13.6</v>
+        <v>12.8</v>
       </c>
       <c r="T159" t="n">
         <v>1.5</v>
@@ -9280,46 +9278,36 @@
         <v>20</v>
       </c>
       <c r="F160" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G160" t="n">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="H160"/>
       <c r="I160"/>
-      <c r="J160" t="n">
-        <v>17</v>
-      </c>
+      <c r="J160"/>
       <c r="K160" t="s">
         <v>51</v>
       </c>
-      <c r="L160" t="s">
-        <v>28</v>
-      </c>
-      <c r="M160" t="n">
-        <v>45</v>
-      </c>
-      <c r="N160" t="n">
-        <v>2</v>
-      </c>
+      <c r="L160"/>
+      <c r="M160"/>
+      <c r="N160"/>
       <c r="O160" t="n">
-        <v>22.22</v>
+        <v>21.11</v>
       </c>
       <c r="P160" t="n">
-        <v>42.84</v>
+        <v>43.74</v>
       </c>
       <c r="Q160" t="n">
-        <v>65.06</v>
+        <v>64.85</v>
       </c>
       <c r="R160" t="n">
-        <v>1634.5</v>
+        <v>1603.5</v>
       </c>
       <c r="S160" t="n">
-        <v>12.8</v>
-      </c>
-      <c r="T160" t="n">
-        <v>1.5</v>
-      </c>
+        <v>13.1</v>
+      </c>
+      <c r="T160"/>
       <c r="U160"/>
     </row>
     <row r="161">
@@ -9339,10 +9327,10 @@
         <v>20</v>
       </c>
       <c r="F161" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G161" t="n">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="H161"/>
       <c r="I161"/>
@@ -9353,66 +9341,17 @@
       <c r="L161"/>
       <c r="M161"/>
       <c r="N161"/>
-      <c r="O161" t="n">
-        <v>21.11</v>
-      </c>
-      <c r="P161" t="n">
-        <v>43.74</v>
-      </c>
-      <c r="Q161" t="n">
-        <v>64.85</v>
-      </c>
+      <c r="O161"/>
+      <c r="P161"/>
+      <c r="Q161"/>
       <c r="R161" t="n">
-        <v>1603.5</v>
+        <v>1864.5</v>
       </c>
       <c r="S161" t="n">
-        <v>13.1</v>
+        <v>11.4</v>
       </c>
       <c r="T161"/>
       <c r="U161"/>
-    </row>
-    <row r="162">
-      <c r="A162" t="s">
-        <v>21</v>
-      </c>
-      <c r="B162" t="s">
-        <v>50</v>
-      </c>
-      <c r="C162" t="n">
-        <v>2021</v>
-      </c>
-      <c r="D162" t="s">
-        <v>49</v>
-      </c>
-      <c r="E162" t="n">
-        <v>20</v>
-      </c>
-      <c r="F162" t="n">
-        <v>4</v>
-      </c>
-      <c r="G162" t="n">
-        <v>67</v>
-      </c>
-      <c r="H162"/>
-      <c r="I162"/>
-      <c r="J162"/>
-      <c r="K162" t="s">
-        <v>51</v>
-      </c>
-      <c r="L162"/>
-      <c r="M162"/>
-      <c r="N162"/>
-      <c r="O162"/>
-      <c r="P162"/>
-      <c r="Q162"/>
-      <c r="R162" t="n">
-        <v>1864.5</v>
-      </c>
-      <c r="S162" t="n">
-        <v>11.4</v>
-      </c>
-      <c r="T162"/>
-      <c r="U162"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>